<commit_message>
v0.41 Few minor adjustments
</commit_message>
<xml_diff>
--- a/DEMO/DEMO_INT_EXT_25.xlsx
+++ b/DEMO/DEMO_INT_EXT_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E\DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008DA7E-0EB6-44DA-A8F0-E61F166C448E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5255335F-3B3E-4B1D-9742-D3BE7EB9D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16665" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="497" activeTab="1" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="85">
   <si>
     <t>Week starts on</t>
   </si>
@@ -223,33 +223,6 @@
     <t>INT - OO- Devops engineer - 3</t>
   </si>
   <si>
-    <t>INT - OO- Devops engineer - 4</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 5</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 6</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 7</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 8</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 9</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 10</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 11</t>
-  </si>
-  <si>
-    <t>INT - OO- Devops engineer - 12</t>
-  </si>
-  <si>
     <t>January</t>
   </si>
   <si>
@@ -302,6 +275,27 @@
   </si>
   <si>
     <t>AU44-PRO0022644</t>
+  </si>
+  <si>
+    <t>Document Date</t>
+  </si>
+  <si>
+    <t>Document type</t>
+  </si>
+  <si>
+    <t>Ref. document number</t>
+  </si>
+  <si>
+    <t>Document Number</t>
+  </si>
+  <si>
+    <t>KV</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>KB</t>
   </si>
 </sst>
 </file>
@@ -499,13 +493,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -513,6 +506,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -837,8 +833,8 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D53"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,10 +898,10 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
-        <v>45663</v>
+        <v>45712</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>32</v>
@@ -917,27 +913,27 @@
         <v>50</v>
       </c>
       <c r="F2" s="30">
-        <v>10</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H2" s="31">
-        <v>750</v>
+        <v>1440</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
-        <v>45670</v>
+        <v>45719</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>32</v>
@@ -949,283 +945,283 @@
         <v>50</v>
       </c>
       <c r="F3" s="30">
-        <v>12</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H3" s="31">
-        <v>900</v>
+        <v>1560</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
-        <v>45677</v>
+        <v>45789</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F4" s="30">
-        <v>14</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>56</v>
+        <v>3</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H4" s="31">
-        <v>1050</v>
+        <v>180</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
-        <v>45684</v>
+        <v>45796</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" s="30">
-        <v>16</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>57</v>
+        <v>4</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H5" s="31">
-        <v>4000</v>
+        <v>240</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
-        <v>45698</v>
+        <v>45859</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F6" s="30">
-        <v>20</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>55</v>
+        <v>17</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H6" s="31">
-        <v>2000</v>
+        <v>1020</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
-        <v>45705</v>
+        <v>45866</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F7" s="30">
-        <v>22</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H7" s="31">
-        <v>2200</v>
+        <v>1140</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <v>45691</v>
+        <v>45929</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F8" s="30">
-        <v>18</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>57</v>
+        <v>5</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H8" s="31">
-        <v>4500</v>
+        <v>300</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <v>45712</v>
+        <v>45936</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F9" s="30">
-        <v>24</v>
-      </c>
-      <c r="G9" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="31">
-        <v>1440</v>
+        <v>360</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
-        <v>45740</v>
+        <v>45999</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F10" s="30">
-        <v>6</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>56</v>
+        <v>15</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H10" s="31">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
-        <v>45747</v>
+        <v>46006</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F11" s="30">
-        <v>8</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H11" s="31">
-        <v>600</v>
+        <v>960</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
-        <v>45719</v>
+        <v>45684</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>32</v>
@@ -1237,27 +1233,27 @@
         <v>50</v>
       </c>
       <c r="F12" s="30">
-        <v>26</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H12" s="31">
-        <v>1560</v>
+        <v>4000</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
-        <v>45726</v>
+        <v>45691</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>32</v>
@@ -1269,59 +1265,59 @@
         <v>50</v>
       </c>
       <c r="F13" s="30">
-        <v>2</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H13" s="31">
-        <v>50</v>
+        <v>4500</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
-        <v>45733</v>
+        <v>45754</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" s="30">
-        <v>4</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H14" s="31">
-        <v>100</v>
+        <v>7000</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
-        <v>45775</v>
+        <v>45761</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>33</v>
@@ -1333,24 +1329,24 @@
         <v>51</v>
       </c>
       <c r="F15" s="30">
-        <v>1</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H15" s="31">
-        <v>100</v>
+        <v>7500</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
-        <v>45754</v>
+        <v>45768</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>39</v>
@@ -1365,347 +1361,347 @@
         <v>51</v>
       </c>
       <c r="F16" s="30">
-        <v>28</v>
-      </c>
-      <c r="G16" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="26" t="s">
         <v>57</v>
       </c>
       <c r="H16" s="31">
-        <v>7000</v>
+        <v>6750</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
-        <v>45761</v>
+        <v>45831</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F17" s="30">
-        <v>30</v>
-      </c>
-      <c r="G17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>57</v>
       </c>
       <c r="H17" s="31">
-        <v>7500</v>
+        <v>2250</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
-        <v>45768</v>
+        <v>45838</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" s="30">
-        <v>27</v>
-      </c>
-      <c r="G18" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="26" t="s">
         <v>57</v>
       </c>
       <c r="H18" s="31">
-        <v>6750</v>
+        <v>2750</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
-        <v>45782</v>
+        <v>45901</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F19" s="30">
-        <v>2</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H19" s="31">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="I19" s="32" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
-        <v>45789</v>
+        <v>45908</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F20" s="30">
-        <v>3</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H20" s="31">
-        <v>180</v>
+        <v>500</v>
       </c>
       <c r="I20" s="32" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
-        <v>45796</v>
+        <v>45971</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F21" s="30">
-        <v>4</v>
-      </c>
-      <c r="G21" s="35" t="s">
-        <v>58</v>
+        <v>11</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H21" s="31">
-        <v>240</v>
+        <v>2750</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
-        <v>45803</v>
+        <v>45978</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F22" s="30">
-        <v>5</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>61</v>
+        <v>12</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="H22" s="31">
-        <v>125</v>
+        <v>3000</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
-        <v>45817</v>
+        <v>45663</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" s="30">
-        <v>7</v>
-      </c>
-      <c r="G23" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H23" s="31">
-        <v>525</v>
+        <v>750</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
-        <v>45824</v>
+        <v>45670</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F24" s="30">
-        <v>8</v>
-      </c>
-      <c r="G24" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="31">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
-        <v>45831</v>
+        <v>45677</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="30">
-        <v>9</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>57</v>
+        <v>14</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H25" s="31">
-        <v>2250</v>
+        <v>1050</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
-        <v>45838</v>
+        <v>45740</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="30">
-        <v>11</v>
-      </c>
-      <c r="G26" s="35" t="s">
-        <v>57</v>
+        <v>6</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H26" s="31">
-        <v>2750</v>
+        <v>450</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J26" s="32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
-        <v>45810</v>
+        <v>45747</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>33</v>
@@ -1717,27 +1713,27 @@
         <v>51</v>
       </c>
       <c r="F27" s="30">
-        <v>6</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>62</v>
+        <v>8</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H27" s="31">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
-        <v>45845</v>
+        <v>45817</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="33" t="s">
         <v>34</v>
@@ -1749,27 +1745,27 @@
         <v>52</v>
       </c>
       <c r="F28" s="30">
-        <v>13</v>
-      </c>
-      <c r="G28" s="35" t="s">
-        <v>55</v>
+        <v>7</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H28" s="31">
-        <v>1300</v>
+        <v>525</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
-        <v>45852</v>
+        <v>45824</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="33" t="s">
         <v>34</v>
@@ -1781,466 +1777,466 @@
         <v>52</v>
       </c>
       <c r="F29" s="30">
-        <v>15</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>55</v>
+        <v>8</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H29" s="31">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
-        <v>45859</v>
+        <v>45887</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F30" s="30">
-        <v>17</v>
-      </c>
-      <c r="G30" s="35" t="s">
-        <v>58</v>
+        <v>25</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H30" s="31">
-        <v>1020</v>
+        <v>1875</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
-        <v>45866</v>
+        <v>45894</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F31" s="30">
-        <v>19</v>
-      </c>
-      <c r="G31" s="35" t="s">
-        <v>58</v>
+        <v>29</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="H31" s="31">
-        <v>1140</v>
+        <v>2175</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
-        <v>45887</v>
+        <v>45957</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F32" s="30">
-        <v>25</v>
-      </c>
-      <c r="G32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H32" s="31">
-        <v>1875</v>
+        <v>675</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
-        <v>45894</v>
+        <v>45964</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F33" s="30">
+        <v>10</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="31">
+        <v>750</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="17">
+        <v>50</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="19">
+        <v>2000</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="31">
-        <v>2175</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
-        <v>45873</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="30">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="17">
+        <v>12</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="19">
+        <v>480</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="17">
+        <v>30</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="19">
+        <v>1500</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>45324</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="11">
+        <v>100</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="13">
+        <v>5000</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>45334</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="11">
+        <v>46</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="13">
+        <v>2300</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="17">
+        <v>124</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="19">
+        <v>6200</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="17">
+        <v>76</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="19">
+        <v>3040</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>45324</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="11">
+        <v>20</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="13">
+        <v>2000</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="17">
         <v>21</v>
       </c>
-      <c r="G34" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H34" s="31">
-        <v>525</v>
-      </c>
-      <c r="I34" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="J34" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
-        <v>45880</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="30">
+      <c r="G42" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="31">
-        <v>575</v>
-      </c>
-      <c r="I35" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="J35" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
-        <v>45915</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="30">
-        <v>3</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="H36" s="31">
-        <v>300</v>
-      </c>
-      <c r="I36" s="32" t="s">
+      <c r="H42" s="19">
+        <v>3150</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J42" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
-        <v>45922</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="30">
-        <v>4</v>
-      </c>
-      <c r="G37" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="H37" s="31">
-        <v>400</v>
-      </c>
-      <c r="I37" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J37" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
-        <v>45901</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="30">
-        <v>1</v>
-      </c>
-      <c r="G38" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="H38" s="31">
-        <v>250</v>
-      </c>
-      <c r="I38" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J38" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
-        <v>45908</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="30">
-        <v>2</v>
-      </c>
-      <c r="G39" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="31">
-        <v>500</v>
-      </c>
-      <c r="I39" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
-        <v>45929</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" s="30">
-        <v>5</v>
-      </c>
-      <c r="G40" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H40" s="31">
-        <v>300</v>
-      </c>
-      <c r="I40" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
-        <v>45957</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="30">
-        <v>9</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="H41" s="31">
-        <v>675</v>
-      </c>
-      <c r="I41" s="32" t="s">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="17">
+        <v>22</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="19">
+        <v>3300</v>
+      </c>
+      <c r="I43" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
-        <v>45936</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="30">
-        <v>6</v>
-      </c>
-      <c r="G42" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" s="31">
-        <v>360</v>
-      </c>
-      <c r="I42" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="J42" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
-        <v>45943</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="30">
-        <v>7</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="H43" s="31">
-        <v>175</v>
-      </c>
-      <c r="I43" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="J43" s="32" t="s">
+      <c r="J43" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2263,8 +2259,8 @@
       <c r="F44" s="30">
         <v>8</v>
       </c>
-      <c r="G44" s="35" t="s">
-        <v>66</v>
+      <c r="G44" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H44" s="31">
         <v>200</v>
@@ -2278,10 +2274,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
-        <v>45985</v>
+        <v>46013</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>36</v>
@@ -2293,27 +2289,27 @@
         <v>54</v>
       </c>
       <c r="F45" s="30">
-        <v>13</v>
-      </c>
-      <c r="G45" s="35" t="s">
-        <v>55</v>
+        <v>17</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H45" s="31">
-        <v>1300</v>
+        <v>425</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="J45" s="32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
-        <v>45964</v>
+        <v>46020</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>36</v>
@@ -2325,569 +2321,569 @@
         <v>54</v>
       </c>
       <c r="F46" s="30">
-        <v>10</v>
-      </c>
-      <c r="G46" s="35" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H46" s="31">
-        <v>750</v>
+        <v>450</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
-        <v>45971</v>
+        <v>45726</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F47" s="30">
-        <v>11</v>
-      </c>
-      <c r="G47" s="35" t="s">
-        <v>57</v>
+        <v>2</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H47" s="31">
-        <v>2750</v>
+        <v>50</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
-        <v>45978</v>
+        <v>45733</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F48" s="30">
-        <v>12</v>
-      </c>
-      <c r="G48" s="35" t="s">
-        <v>57</v>
+        <v>4</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H48" s="31">
-        <v>3000</v>
+        <v>100</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
-        <v>45992</v>
+        <v>45803</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F49" s="30">
-        <v>14</v>
-      </c>
-      <c r="G49" s="35" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H49" s="31">
-        <v>1400</v>
+        <v>125</v>
       </c>
       <c r="I49" s="32" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="J49" s="32" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
-        <v>45999</v>
+        <v>45810</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F50" s="30">
-        <v>15</v>
-      </c>
-      <c r="G50" s="35" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H50" s="31">
-        <v>900</v>
+        <v>150</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="J50" s="32" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
-        <v>46006</v>
+        <v>45873</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F51" s="30">
-        <v>16</v>
-      </c>
-      <c r="G51" s="35" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H51" s="31">
-        <v>960</v>
+        <v>525</v>
       </c>
       <c r="I51" s="32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J51" s="32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
-        <v>46013</v>
+        <v>45880</v>
       </c>
       <c r="B52" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F52" s="30">
-        <v>17</v>
-      </c>
-      <c r="G52" s="35" t="s">
-        <v>67</v>
+        <v>23</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="H52" s="31">
-        <v>425</v>
+        <v>575</v>
       </c>
       <c r="I52" s="32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J52" s="32" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
-        <v>46020</v>
+        <v>45943</v>
       </c>
       <c r="B53" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C53" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" s="30">
+        <v>7</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="31">
+        <v>175</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="27">
+        <v>45698</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="30">
+        <v>20</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" s="31">
+        <v>2000</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="27">
+        <v>45705</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="30">
+        <v>22</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H55" s="31">
+        <v>2200</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="27">
+        <v>45775</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" s="30">
+        <v>1</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="31">
+        <v>100</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J56" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="27">
+        <v>45782</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="30">
+        <v>2</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H57" s="31">
+        <v>200</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="J57" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="27">
+        <v>45845</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="30">
+        <v>13</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H58" s="31">
+        <v>1300</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="J58" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="27">
+        <v>45852</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="30">
+        <v>15</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59" s="31">
+        <v>1500</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="J59" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="27">
+        <v>45915</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F60" s="30">
+        <v>3</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H60" s="31">
+        <v>300</v>
+      </c>
+      <c r="I60" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="27">
+        <v>45922</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" s="30">
+        <v>4</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61" s="31">
+        <v>400</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="27">
+        <v>45985</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D62" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E62" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="30">
-        <v>18</v>
-      </c>
-      <c r="G53" s="35" t="s">
+      <c r="F62" s="30">
+        <v>13</v>
+      </c>
+      <c r="G62" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H62" s="31">
+        <v>1300</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J62" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="27">
+        <v>45992</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" s="30">
+        <v>14</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="31">
+        <v>1400</v>
+      </c>
+      <c r="I63" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H53" s="31">
-        <v>450</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="J53" s="32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
-        <v>45324</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="11">
-        <v>20</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="13">
-        <v>2000</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J54" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
-        <v>45324</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="11">
-        <v>100</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="13">
-        <v>5000</v>
-      </c>
-      <c r="I55" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
-        <v>45334</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="11">
-        <v>46</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="13">
-        <v>2300</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J56" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="17">
-        <v>124</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="19">
-        <v>6200</v>
-      </c>
-      <c r="I57" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J57" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="17">
-        <v>50</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H58" s="19">
-        <v>2000</v>
-      </c>
-      <c r="I58" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J58" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="17">
-        <v>21</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H59" s="19">
-        <v>3150</v>
-      </c>
-      <c r="I59" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="17">
-        <v>12</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H60" s="19">
-        <v>480</v>
-      </c>
-      <c r="I60" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J60" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="17">
-        <v>76</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="19">
-        <v>3040</v>
-      </c>
-      <c r="I61" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J61" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" s="17">
-        <v>30</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="19">
-        <v>1500</v>
-      </c>
-      <c r="I62" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J62" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="17">
-        <v>22</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H63" s="19">
-        <v>3300</v>
-      </c>
-      <c r="I63" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J63" s="20" t="s">
-        <v>28</v>
+      <c r="J63" s="32" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J11" xr:uid="{71860C13-2C7C-4F48-80B3-9582C9C756CA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J63">
-      <sortCondition ref="I1:I11"/>
+      <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2900,11 +2896,11 @@
   <sheetPr codeName="Blad2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2914,11 +2910,15 @@
     <col min="3" max="3" width="23.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="6" max="6" width="12.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -2934,11 +2934,23 @@
       <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2954,11 +2966,23 @@
       <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="37">
-        <v>42308.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="36">
+        <v>-42308.6</v>
+      </c>
+      <c r="G2" s="38">
+        <v>45736</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="6">
+        <v>43871865021</v>
+      </c>
+      <c r="J2" s="6">
+        <v>34450409398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2024</v>
       </c>
@@ -2974,11 +2998,23 @@
       <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="36">
         <v>-111830</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="38">
+        <v>45578</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="6">
+        <v>45173004338</v>
+      </c>
+      <c r="J3" s="6">
+        <v>21400037218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2025</v>
       </c>
@@ -2986,19 +3022,31 @@
         <v>1</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="38">
+        <v>69</v>
+      </c>
+      <c r="F4" s="37">
         <v>9040.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="38">
+        <v>45673</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="6">
+        <v>84942245989</v>
+      </c>
+      <c r="J4" s="6">
+        <v>19721046273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2025</v>
       </c>
@@ -3006,19 +3054,31 @@
         <v>2</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>46</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="38">
+        <v>70</v>
+      </c>
+      <c r="F5" s="37">
         <v>4826.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="38">
+        <v>45691</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="6">
+        <v>67336419499</v>
+      </c>
+      <c r="J5" s="6">
+        <v>18531963987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2025</v>
       </c>
@@ -3026,19 +3086,31 @@
         <v>4</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="38">
+        <v>71</v>
+      </c>
+      <c r="F6" s="37">
         <v>4613.1099999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="38">
+        <v>45761</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="6">
+        <v>15094735521</v>
+      </c>
+      <c r="J6" s="6">
+        <v>15132027714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2025</v>
       </c>
@@ -3046,19 +3118,31 @@
         <v>5</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="38">
+        <v>72</v>
+      </c>
+      <c r="F7" s="37">
         <v>4984.33</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="38">
+        <v>45788</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="6">
+        <v>65032179863</v>
+      </c>
+      <c r="J7" s="6">
+        <v>71740212896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2025</v>
       </c>
@@ -3066,19 +3150,31 @@
         <v>6</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="38">
+        <v>69</v>
+      </c>
+      <c r="F8" s="37">
         <v>2641.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="38">
+        <v>45832</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="6">
+        <v>62144195021</v>
+      </c>
+      <c r="J8" s="6">
+        <v>16256005023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2025</v>
       </c>
@@ -3086,19 +3182,31 @@
         <v>7</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="38">
+        <v>70</v>
+      </c>
+      <c r="F9" s="37">
         <v>6800.47</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="38">
+        <v>45862</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="6">
+        <v>46986506059</v>
+      </c>
+      <c r="J9" s="6">
+        <v>87236234494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2025</v>
       </c>
@@ -3106,19 +3214,31 @@
         <v>8</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="38">
+        <v>71</v>
+      </c>
+      <c r="F10" s="37">
         <v>7903.82</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="38">
+        <v>45870</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="6">
+        <v>36324782342</v>
+      </c>
+      <c r="J10" s="6">
+        <v>27314698694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2025</v>
       </c>
@@ -3126,19 +3246,31 @@
         <v>9</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="38">
+        <v>72</v>
+      </c>
+      <c r="F11" s="37">
         <v>6495.84</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="38">
+        <v>45907</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="6">
+        <v>78193897676</v>
+      </c>
+      <c r="J11" s="6">
+        <v>91610896112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2025</v>
       </c>
@@ -3146,19 +3278,31 @@
         <v>10</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="38">
+        <v>69</v>
+      </c>
+      <c r="F12" s="37">
         <v>3190.13</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="38">
+        <v>45932</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="6">
+        <v>54804135807</v>
+      </c>
+      <c r="J12" s="6">
+        <v>70234515409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>2025</v>
       </c>
@@ -3166,19 +3310,31 @@
         <v>11</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="38">
+        <v>70</v>
+      </c>
+      <c r="F13" s="37">
         <v>3543.82</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="38">
+        <v>45972</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="6">
+        <v>47210725852</v>
+      </c>
+      <c r="J13" s="6">
+        <v>54245469062</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2025</v>
       </c>
@@ -3186,19 +3342,31 @@
         <v>12</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="38">
+        <v>71</v>
+      </c>
+      <c r="F14" s="37">
         <v>1870.91</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="38">
+        <v>46022</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="6">
+        <v>93761401475</v>
+      </c>
+      <c r="J14" s="6">
+        <v>16220208557</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2024</v>
       </c>
@@ -3206,19 +3374,31 @@
         <v>1</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="38">
+        <v>72</v>
+      </c>
+      <c r="F15" s="37">
         <v>8662.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="38">
+        <v>45673</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="6">
+        <v>32924431579</v>
+      </c>
+      <c r="J15" s="6">
+        <v>72065727213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>2024</v>
       </c>
@@ -3226,19 +3406,31 @@
         <v>2</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="38">
+        <v>69</v>
+      </c>
+      <c r="F16" s="37">
         <v>3199.15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="38">
+        <v>45691</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="6">
+        <v>57054367324</v>
+      </c>
+      <c r="J16" s="6">
+        <v>6361519091</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>2024</v>
       </c>
@@ -3246,19 +3438,31 @@
         <v>3</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="38">
+        <v>70</v>
+      </c>
+      <c r="F17" s="37">
         <v>3752.02</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="38">
+        <v>45719</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="6">
+        <v>71060016504</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1183636558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2024</v>
       </c>
@@ -3266,19 +3470,31 @@
         <v>4</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="38">
+        <v>71</v>
+      </c>
+      <c r="F18" s="37">
         <v>9634.85</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="38">
+        <v>45761</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="6">
+        <v>761520322</v>
+      </c>
+      <c r="J18" s="6">
+        <v>32918208331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>2024</v>
       </c>
@@ -3286,19 +3502,31 @@
         <v>5</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D19" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="38">
+        <v>72</v>
+      </c>
+      <c r="F19" s="37">
         <v>7958.62</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="38">
+        <v>45788</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="6">
+        <v>7204455075</v>
+      </c>
+      <c r="J19" s="6">
+        <v>68102934492</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>2024</v>
       </c>
@@ -3306,19 +3534,31 @@
         <v>6</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D20" s="29" t="s">
         <v>46</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="38">
+        <v>69</v>
+      </c>
+      <c r="F20" s="37">
         <v>4683.7700000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="38">
+        <v>45832</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="6">
+        <v>15781316352</v>
+      </c>
+      <c r="J20" s="6">
+        <v>50343815462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>2024</v>
       </c>
@@ -3326,19 +3566,31 @@
         <v>7</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="38">
+        <v>70</v>
+      </c>
+      <c r="F21" s="37">
         <v>7106.73</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="38">
+        <v>45862</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="6">
+        <v>96965559273</v>
+      </c>
+      <c r="J21" s="6">
+        <v>25596364417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>2024</v>
       </c>
@@ -3346,19 +3598,31 @@
         <v>8</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D22" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="38">
+        <v>71</v>
+      </c>
+      <c r="F22" s="37">
         <v>667.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="38">
+        <v>45870</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="6">
+        <v>49797764506</v>
+      </c>
+      <c r="J22" s="6">
+        <v>10983569653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>2024</v>
       </c>
@@ -3366,19 +3630,31 @@
         <v>9</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="38">
+        <v>72</v>
+      </c>
+      <c r="F23" s="37">
         <v>905.46</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="38">
+        <v>45907</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="6">
+        <v>94470446773</v>
+      </c>
+      <c r="J23" s="6">
+        <v>90893677197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>2024</v>
       </c>
@@ -3386,31 +3662,43 @@
         <v>11</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="38">
+        <v>72</v>
+      </c>
+      <c r="F24" s="37">
         <v>1169.6199999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="38">
+        <v>45991</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="6">
+        <v>16830570217</v>
+      </c>
+      <c r="J24" s="6">
+        <v>40811527608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
     </row>
@@ -3421,6 +3709,99 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
+      <Description>RPRC6KRT5W67-1044406188-39062</Description>
+    </_dlc_DocIdUrl>
+    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g9f43ae49e884a1b9be7dc5d6f9369ce>
+    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </DossierOwner>
+    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gd3cfa1af6a84b6687f5776992485533>
+    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FFB3B7DE9242943AFC83F55587E815F" ma:contentTypeVersion="332" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa82c5eea78b7e638bce7457d0c1ee6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f1f29378-94b6-4af4-bdac-5601381a5dad" xmlns:ns3="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="361f62c40be1fed3631387308499c1cb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3724,100 +4105,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
-      <Description>RPRC6KRT5W67-1044406188-39062</Description>
-    </_dlc_DocIdUrl>
-    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g9f43ae49e884a1b9be7dc5d6f9369ce>
-    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </DossierOwner>
-    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gd3cfa1af6a84b6687f5776992485533>
-    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF78F3BA-2CB7-4081-98E3-62DAC42A3FA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3835,38 +4157,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v0.46 Added detailed invoice tabs in export to excel
</commit_message>
<xml_diff>
--- a/DEMO/DEMO_INT_EXT_25.xlsx
+++ b/DEMO/DEMO_INT_EXT_25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E_web\DEMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E\DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934C76A9-B81D-4F46-8287-AD183B21FCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCF50D7-85C6-4E9E-B3EA-08955A81CAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="497" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="497" activeTab="1" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
   </bookViews>
   <sheets>
     <sheet name="PPM - All details" sheetId="11" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>Optimus Prime</t>
   </si>
   <si>
-    <t>Arche Bunker</t>
-  </si>
-  <si>
     <t>Snowwhite</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>CTC</t>
+  </si>
+  <si>
+    <t>Archie Bunker</t>
   </si>
 </sst>
 </file>
@@ -871,9 +871,9 @@
   </sheetPr>
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,13 +928,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
@@ -946,22 +946,22 @@
         <v>45698</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="30">
         <v>20</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="31">
         <v>2000</v>
@@ -973,13 +973,13 @@
         <v>12</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -987,22 +987,22 @@
         <v>45705</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="30">
         <v>22</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" s="31">
         <v>2200</v>
@@ -1014,24 +1014,24 @@
         <v>12</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
-        <v>45663</v>
+        <v>45775</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>45</v>
@@ -1040,25 +1040,25 @@
         <v>50</v>
       </c>
       <c r="F4" s="30">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4" s="31">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M4" s="26" t="s">
         <v>96</v>
@@ -1066,13 +1066,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
-        <v>45670</v>
+        <v>45782</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>45</v>
@@ -1081,25 +1081,25 @@
         <v>50</v>
       </c>
       <c r="F5" s="30">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" s="31">
-        <v>900</v>
+        <v>200</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M5" s="26" t="s">
         <v>96</v>
@@ -1107,40 +1107,40 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
-        <v>45677</v>
+        <v>45915</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="30">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H6" s="31">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M6" s="26" t="s">
         <v>96</v>
@@ -1148,40 +1148,40 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
-        <v>45684</v>
+        <v>45922</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="30">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H7" s="31">
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>96</v>
@@ -1189,40 +1189,40 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <v>45691</v>
+        <v>45985</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="30">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H8" s="31">
-        <v>4500</v>
+        <v>1300</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>96</v>
@@ -1230,40 +1230,40 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <v>45712</v>
+        <v>45992</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" s="30">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H9" s="31">
-        <v>1440</v>
+        <v>1400</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M9" s="26" t="s">
         <v>96</v>
@@ -1271,122 +1271,118 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
-        <v>45719</v>
+        <v>45845</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F10" s="30">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H10" s="31">
-        <v>1560</v>
+        <f>1300*1</f>
+        <v>1300</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L10" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M10" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
-        <v>45726</v>
+        <v>45852</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" s="30">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H11" s="31">
-        <v>50</v>
+        <f>1500*1</f>
+        <v>1500</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K11" s="26" t="s">
         <v>92</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M11" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
-        <v>45733</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="29" t="s">
+      <c r="A12" s="15">
+        <v>45592</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="17">
         <v>50</v>
       </c>
-      <c r="F12" s="30">
-        <v>4</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="31">
-        <v>100</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>60</v>
+      <c r="G12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="19">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M12" s="26" t="s">
         <v>96</v>
@@ -1409,28 +1405,28 @@
         <v>11</v>
       </c>
       <c r="F13" s="17">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="19">
-        <v>2000</v>
+        <v>480</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M13" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1450,13 +1446,13 @@
         <v>11</v>
       </c>
       <c r="F14" s="17">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="19">
-        <v>480</v>
+        <v>1500</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>28</v>
@@ -1465,13 +1461,13 @@
         <v>28</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M14" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1491,28 +1487,28 @@
         <v>11</v>
       </c>
       <c r="F15" s="17">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H15" s="19">
-        <v>1500</v>
+        <v>6200</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M15" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1532,28 +1528,28 @@
         <v>11</v>
       </c>
       <c r="F16" s="17">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="19">
-        <v>6200</v>
+        <v>3040</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1573,28 +1569,28 @@
         <v>11</v>
       </c>
       <c r="F17" s="17">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="19">
-        <v>3040</v>
+        <v>3150</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M17" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1614,818 +1610,814 @@
         <v>11</v>
       </c>
       <c r="F18" s="17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="19">
-        <v>3150</v>
+        <v>3300</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <v>45592</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="17">
-        <v>22</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="19">
-        <v>3300</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>28</v>
+      <c r="A19" s="27">
+        <v>45663</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="30">
+        <v>10</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="31">
+        <v>750</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M19" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>45324</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="27">
+        <v>45670</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="11">
-        <v>20</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="13">
-        <v>2000</v>
-      </c>
-      <c r="I20" s="14" t="s">
+      <c r="E20" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="30">
         <v>12</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>12</v>
+      <c r="G20" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="31">
+        <v>900</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M20" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>45324</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="11">
-        <v>100</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="13">
-        <v>5000</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>12</v>
+      <c r="A21" s="27">
+        <v>45677</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="30">
+        <v>14</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="31">
+        <v>1050</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M21" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>45334</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="11">
-        <v>46</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="13">
-        <v>2300</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>12</v>
+      <c r="A22" s="27">
+        <v>45740</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="30">
+        <v>6</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="31">
+        <v>450</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>59</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M22" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
-        <v>45775</v>
+        <v>45747</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="30">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G23" s="26" t="s">
         <v>54</v>
       </c>
       <c r="H23" s="31">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M23" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
-        <v>45782</v>
+        <v>45887</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="30">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="G24" s="26" t="s">
         <v>54</v>
       </c>
       <c r="H24" s="31">
-        <v>200</v>
+        <v>1875</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L24" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M24" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
-        <v>45740</v>
+        <v>45894</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="30">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="31">
-        <v>450</v>
+        <v>2175</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L25" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M25" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
-        <v>45747</v>
+        <v>45957</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F26" s="30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H26" s="31">
-        <v>600</v>
+        <v>675</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="J26" s="32" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L26" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M26" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
-        <v>45754</v>
+        <v>45964</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F27" s="30">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H27" s="31">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L27" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M27" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
-        <v>45761</v>
+        <v>45817</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="F28" s="30">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H28" s="31">
-        <v>7500</v>
+        <f>525*1</f>
+        <v>525</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K28" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L28" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="M28" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="M28" s="26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
-        <v>45768</v>
+        <v>45824</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="F29" s="30">
+        <v>8</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="31">
+        <f>600*1</f>
+        <v>600</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="M29" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>45324</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="31">
-        <v>6750</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="J29" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="L29" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="M29" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
-        <v>45789</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="30">
-        <v>3</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="31">
-        <v>180</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" s="32" t="s">
-        <v>62</v>
+      <c r="E30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="11">
+        <v>20</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="13">
+        <v>2000</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M30" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
-        <v>45796</v>
+        <v>45684</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F31" s="30">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H31" s="31">
-        <v>240</v>
+        <v>4000</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L31" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M31" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
-        <v>45803</v>
+        <v>45691</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F32" s="30">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H32" s="31">
-        <v>125</v>
+        <v>4500</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L32" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M32" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
-        <v>45810</v>
+        <v>45754</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="30">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H33" s="31">
-        <v>150</v>
+        <v>7000</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L33" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M33" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
-        <v>45915</v>
+        <v>45761</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F34" s="30">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H34" s="31">
-        <v>300</v>
+        <v>7500</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="L34" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M34" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
-        <v>45922</v>
+        <v>45768</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F35" s="30">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H35" s="31">
-        <v>400</v>
+        <v>6750</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="K35" s="26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="L35" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M35" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
-        <v>45887</v>
+        <v>45901</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F36" s="30">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G36" s="26" t="s">
         <v>55</v>
       </c>
       <c r="H36" s="31">
-        <v>1875</v>
+        <v>250</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="K36" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L36" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M36" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
-        <v>45894</v>
+        <v>45908</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="30">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="G37" s="26" t="s">
         <v>55</v>
       </c>
       <c r="H37" s="31">
-        <v>2175</v>
+        <v>500</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="K37" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L37" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M37" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
-        <v>45901</v>
+        <v>45971</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>48</v>
@@ -2434,39 +2426,39 @@
         <v>52</v>
       </c>
       <c r="F38" s="30">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H38" s="31">
-        <v>250</v>
+        <v>2750</v>
       </c>
       <c r="I38" s="32" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="J38" s="32" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="K38" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L38" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M38" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
-        <v>45908</v>
+        <v>45978</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>48</v>
@@ -2475,438 +2467,433 @@
         <v>52</v>
       </c>
       <c r="F39" s="30">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H39" s="31">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L39" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M39" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
-        <v>45929</v>
+        <v>45831</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F40" s="30">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H40" s="31">
-        <v>300</v>
+        <f>2250*1</f>
+        <v>2250</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L40" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M40" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
-        <v>45936</v>
+        <v>45838</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F41" s="30">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G41" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H41" s="31">
-        <v>360</v>
+        <v>2750</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="J41" s="32" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="K41" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L41" s="26" t="s">
         <v>94</v>
       </c>
       <c r="M41" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
-        <v>45950</v>
-      </c>
-      <c r="B42" s="29" t="s">
+      <c r="A42" s="7">
+        <v>45324</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="30">
-        <v>8</v>
-      </c>
-      <c r="G42" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H42" s="31">
-        <v>200</v>
-      </c>
-      <c r="I42" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="J42" s="32" t="s">
-        <v>28</v>
+      <c r="C42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="11">
+        <v>100</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="13">
+        <v>5000</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="K42" s="26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L42" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M42" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
-        <v>45943</v>
-      </c>
-      <c r="B43" s="29" t="s">
+      <c r="A43" s="7">
+        <v>45334</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="30">
-        <v>7</v>
-      </c>
-      <c r="G43" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H43" s="31">
-        <v>175</v>
-      </c>
-      <c r="I43" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="J43" s="32" t="s">
-        <v>28</v>
+      <c r="C43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="11">
+        <v>46</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="13">
+        <v>2300</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="K43" s="26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L43" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M43" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
-        <v>45985</v>
+        <v>45712</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D44" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="29" t="s">
-        <v>53</v>
-      </c>
       <c r="F44" s="30">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G44" s="26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H44" s="31">
-        <v>1300</v>
+        <v>1440</v>
       </c>
       <c r="I44" s="32" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L44" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M44" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
-        <v>45992</v>
+        <v>45719</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D45" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="29" t="s">
-        <v>53</v>
-      </c>
       <c r="F45" s="30">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G45" s="26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H45" s="31">
-        <v>1400</v>
+        <v>1560</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J45" s="32" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L45" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M45" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
-        <v>45957</v>
+        <v>45789</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F46" s="30">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H46" s="31">
-        <v>675</v>
+        <v>180</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="K46" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L46" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M46" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
-        <v>45964</v>
+        <v>45796</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F47" s="30">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G47" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H47" s="31">
-        <v>750</v>
+        <v>240</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K47" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L47" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M47" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
-        <v>45971</v>
+        <v>45929</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F48" s="30">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H48" s="31">
-        <v>2750</v>
+        <v>300</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="K48" s="26" t="s">
         <v>86</v>
       </c>
       <c r="L48" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M48" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
-        <v>45978</v>
+        <v>45936</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F49" s="30">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G49" s="26" t="s">
         <v>56</v>
       </c>
       <c r="H49" s="31">
-        <v>3000</v>
+        <v>360</v>
       </c>
       <c r="I49" s="32" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="J49" s="32" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="K49" s="26" t="s">
         <v>86</v>
       </c>
       <c r="L49" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M49" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2914,40 +2901,40 @@
         <v>45999</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F50" s="30">
         <v>15</v>
       </c>
       <c r="G50" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H50" s="31">
         <v>900</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J50" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K50" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L50" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M50" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2955,236 +2942,236 @@
         <v>46006</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F51" s="30">
         <v>16</v>
       </c>
       <c r="G51" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H51" s="31">
         <v>960</v>
       </c>
       <c r="I51" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J51" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L51" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M51" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
-        <v>46013</v>
+        <v>45859</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F52" s="30">
         <v>17</v>
       </c>
       <c r="G52" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H52" s="31">
-        <v>425</v>
+        <v>1020</v>
       </c>
       <c r="I52" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J52" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K52" s="26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L52" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M52" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
-        <v>46020</v>
+        <v>45866</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F53" s="30">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H53" s="31">
-        <v>450</v>
+        <v>1140</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J53" s="32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K53" s="26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L53" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M53" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
-        <v>45845</v>
+        <v>45726</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="F54" s="30">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G54" s="26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H54" s="31">
-        <f>1300*1</f>
-        <v>1300</v>
+        <v>50</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J54" s="32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L54" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M54" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
-        <v>45852</v>
+        <v>45733</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="F55" s="30">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H55" s="31">
-        <f>1500*1</f>
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J55" s="32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K55" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L55" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M55" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
-        <v>45817</v>
+        <v>45803</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="F56" s="30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H56" s="31">
-        <f>525*1</f>
-        <v>525</v>
+        <v>125</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J56" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K56" s="26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L56" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M56" s="26" t="s">
         <v>96</v>
@@ -3192,38 +3179,40 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
-        <v>45824</v>
+        <v>45810</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="F57" s="30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H57" s="31">
-        <f>600*1</f>
-        <v>600</v>
+        <v>150</v>
       </c>
       <c r="I57" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J57" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K57" s="26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L57" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M57" s="26" t="s">
         <v>96</v>
@@ -3231,38 +3220,40 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
-        <v>45831</v>
+        <v>45950</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D58" s="29" t="s">
         <v>47</v>
       </c>
+      <c r="E58" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="F58" s="30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H58" s="31">
-        <f>2250*1</f>
-        <v>2250</v>
+        <v>200</v>
       </c>
       <c r="I58" s="32" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="J58" s="32" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L58" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M58" s="26" t="s">
         <v>96</v>
@@ -3270,37 +3261,40 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
-        <v>45838</v>
+        <v>45943</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D59" s="29" t="s">
         <v>47</v>
       </c>
+      <c r="E59" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="F59" s="30">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H59" s="31">
-        <v>2750</v>
+        <v>175</v>
       </c>
       <c r="I59" s="32" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="J59" s="32" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="K59" s="26" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L59" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M59" s="26" t="s">
         <v>96</v>
@@ -3308,16 +3302,19 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
-        <v>45859</v>
+        <v>46013</v>
       </c>
       <c r="B60" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="F60" s="30">
         <v>17</v>
@@ -3326,19 +3323,19 @@
         <v>57</v>
       </c>
       <c r="H60" s="31">
-        <v>1020</v>
+        <v>425</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J60" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K60" s="26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L60" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M60" s="26" t="s">
         <v>96</v>
@@ -3346,37 +3343,40 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
-        <v>45866</v>
+        <v>46020</v>
       </c>
       <c r="B61" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="F61" s="30">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G61" s="26" t="s">
         <v>57</v>
       </c>
       <c r="H61" s="31">
-        <v>1140</v>
+        <v>450</v>
       </c>
       <c r="I61" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J61" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L61" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M61" s="26" t="s">
         <v>96</v>
@@ -3387,37 +3387,37 @@
         <v>45873</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C62" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F62" s="30">
         <v>21</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H62" s="31">
         <v>525</v>
       </c>
       <c r="I62" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J62" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K62" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L62" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M62" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3425,41 +3425,45 @@
         <v>45880</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F63" s="30">
         <v>23</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H63" s="31">
         <v>575</v>
       </c>
       <c r="I63" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J63" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L63" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M63" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M63" xr:uid="{71860C13-2C7C-4F48-80B3-9582C9C756CA}"/>
+  <autoFilter ref="A1:M63" xr:uid="{71860C13-2C7C-4F48-80B3-9582C9C756CA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M63">
+      <sortCondition ref="B1:B63"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3472,9 +3476,9 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3512,16 +3516,16 @@
         <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3532,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="37">
         <v>9040.9</v>
@@ -3547,7 +3551,7 @@
         <v>45736</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="6">
         <v>43871865021</v>
@@ -3564,13 +3568,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="37">
         <v>6800.47</v>
@@ -3579,7 +3583,7 @@
         <v>45578</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="6">
         <v>45173004338</v>
@@ -3596,13 +3600,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="37">
         <v>1870.91</v>
@@ -3611,7 +3615,7 @@
         <v>45673</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" s="6">
         <v>84942245989</v>
@@ -3628,13 +3632,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="37">
         <v>7958.62</v>
@@ -3643,7 +3647,7 @@
         <v>45691</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="6">
         <v>67336419499</v>
@@ -3660,13 +3664,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="37">
         <v>1169.6199999999999</v>
@@ -3675,7 +3679,7 @@
         <v>45761</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="6">
         <v>15094735521</v>
@@ -3707,7 +3711,7 @@
         <v>45788</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="6">
         <v>65032179863</v>
@@ -3739,7 +3743,7 @@
         <v>45832</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="6">
         <v>62144195021</v>
@@ -3756,13 +3760,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="37">
         <v>4826.2</v>
@@ -3771,7 +3775,7 @@
         <v>45862</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="6">
         <v>46986506059</v>
@@ -3788,13 +3792,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="37">
         <v>7903.82</v>
@@ -3803,7 +3807,7 @@
         <v>45870</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="6">
         <v>36324782342</v>
@@ -3820,13 +3824,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="37">
         <v>8662.9</v>
@@ -3835,7 +3839,7 @@
         <v>45907</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" s="6">
         <v>78193897676</v>
@@ -3852,13 +3856,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="37">
         <v>4683.7700000000004</v>
@@ -3867,7 +3871,7 @@
         <v>45932</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="6">
         <v>54804135807</v>
@@ -3884,13 +3888,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="37">
         <v>4984.33</v>
@@ -3899,7 +3903,7 @@
         <v>45972</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I13" s="6">
         <v>47210725852</v>
@@ -3916,13 +3920,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="37">
         <v>3190.13</v>
@@ -3931,7 +3935,7 @@
         <v>46022</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" s="6">
         <v>93761401475</v>
@@ -3948,13 +3952,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="37">
         <v>3752.02</v>
@@ -3963,7 +3967,7 @@
         <v>45673</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15" s="6">
         <v>32924431579</v>
@@ -3980,13 +3984,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="37">
         <v>667.1</v>
@@ -3995,7 +3999,7 @@
         <v>45691</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I16" s="6">
         <v>57054367324</v>
@@ -4012,13 +4016,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="37">
         <v>2641.11</v>
@@ -4027,7 +4031,7 @@
         <v>45719</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I17" s="6">
         <v>71060016504</v>
@@ -4044,13 +4048,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="37">
         <v>3543.82</v>
@@ -4059,7 +4063,7 @@
         <v>45761</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="6">
         <v>761520322</v>
@@ -4076,13 +4080,13 @@
         <v>4</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="37">
         <v>9634.85</v>
@@ -4091,7 +4095,7 @@
         <v>45788</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I19" s="6">
         <v>7204455075</v>
@@ -4108,22 +4112,23 @@
         <v>9</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="37">
+        <f>905.46*1</f>
         <v>905.46</v>
       </c>
       <c r="G20" s="38">
         <v>45832</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I20" s="6">
         <v>15781316352</v>
@@ -4143,10 +4148,10 @@
         <v>34</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="37">
         <v>4613.1099999999997</v>
@@ -4155,7 +4160,7 @@
         <v>45862</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="6">
         <v>96965559273</v>
@@ -4175,10 +4180,10 @@
         <v>34</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="37">
         <v>6495.84</v>
@@ -4187,7 +4192,7 @@
         <v>45870</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I22" s="6">
         <v>49797764506</v>
@@ -4207,10 +4212,10 @@
         <v>34</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" s="37">
         <v>3199.15</v>
@@ -4219,7 +4224,7 @@
         <v>45907</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I23" s="6">
         <v>94470446773</v>
@@ -4239,10 +4244,10 @@
         <v>34</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" s="37">
         <v>5000</v>
@@ -4251,7 +4256,7 @@
         <v>45860</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="6">
         <v>16830570217</v>
@@ -4287,6 +4292,99 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
+      <Description>RPRC6KRT5W67-1044406188-39062</Description>
+    </_dlc_DocIdUrl>
+    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g9f43ae49e884a1b9be7dc5d6f9369ce>
+    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </DossierOwner>
+    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gd3cfa1af6a84b6687f5776992485533>
+    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FFB3B7DE9242943AFC83F55587E815F" ma:contentTypeVersion="332" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa82c5eea78b7e638bce7457d0c1ee6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f1f29378-94b6-4af4-bdac-5601381a5dad" xmlns:ns3="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="361f62c40be1fed3631387308499c1cb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4590,100 +4688,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
-      <Description>RPRC6KRT5W67-1044406188-39062</Description>
-    </_dlc_DocIdUrl>
-    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g9f43ae49e884a1b9be7dc5d6f9369ce>
-    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </DossierOwner>
-    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gd3cfa1af6a84b6687f5776992485533>
-    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF78F3BA-2CB7-4081-98E3-62DAC42A3FA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4701,38 +4740,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v0.49 Fix ISO week
</commit_message>
<xml_diff>
--- a/DEMO/DEMO_INT_EXT_25.xlsx
+++ b/DEMO/DEMO_INT_EXT_25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E_web\DEMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E\DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546A248F-59EB-4995-AEEE-8396D9837D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE809C33-A17C-4740-ABF5-AC837A536BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="497" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -446,88 +446,91 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -852,8 +855,8 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3346,11 +3349,11 @@
       <c r="H61" s="11">
         <v>450</v>
       </c>
-      <c r="I61" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>66</v>
+      <c r="I61" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J61" s="31" t="s">
+        <v>58</v>
       </c>
       <c r="K61" s="10" t="s">
         <v>91</v>
@@ -4273,6 +4276,99 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
+      <Description>RPRC6KRT5W67-1044406188-39062</Description>
+    </_dlc_DocIdUrl>
+    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g9f43ae49e884a1b9be7dc5d6f9369ce>
+    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </DossierOwner>
+    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gd3cfa1af6a84b6687f5776992485533>
+    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FFB3B7DE9242943AFC83F55587E815F" ma:contentTypeVersion="332" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa82c5eea78b7e638bce7457d0c1ee6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f1f29378-94b6-4af4-bdac-5601381a5dad" xmlns:ns3="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="361f62c40be1fed3631387308499c1cb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4576,100 +4672,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
-      <Description>RPRC6KRT5W67-1044406188-39062</Description>
-    </_dlc_DocIdUrl>
-    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g9f43ae49e884a1b9be7dc5d6f9369ce>
-    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </DossierOwner>
-    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gd3cfa1af6a84b6687f5776992485533>
-    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF78F3BA-2CB7-4081-98E3-62DAC42A3FA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4687,38 +4724,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v0.51 Fix filter PPM cost=0 undone
</commit_message>
<xml_diff>
--- a/DEMO/DEMO_INT_EXT_25.xlsx
+++ b/DEMO/DEMO_INT_EXT_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E\DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE809C33-A17C-4740-ABF5-AC837A536BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60C89A0-331F-4122-8E39-C8594E6A4773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="497" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3305,9 +3305,7 @@
       <c r="G60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H60" s="11">
-        <v>425</v>
-      </c>
+      <c r="H60" s="1"/>
       <c r="I60" s="12" t="s">
         <v>66</v>
       </c>
@@ -4276,99 +4274,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
-      <Description>RPRC6KRT5W67-1044406188-39062</Description>
-    </_dlc_DocIdUrl>
-    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g9f43ae49e884a1b9be7dc5d6f9369ce>
-    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </DossierOwner>
-    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gd3cfa1af6a84b6687f5776992485533>
-    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FFB3B7DE9242943AFC83F55587E815F" ma:contentTypeVersion="332" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa82c5eea78b7e638bce7457d0c1ee6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f1f29378-94b6-4af4-bdac-5601381a5dad" xmlns:ns3="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="361f62c40be1fed3631387308499c1cb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4672,41 +4577,100 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
+      <Description>RPRC6KRT5W67-1044406188-39062</Description>
+    </_dlc_DocIdUrl>
+    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g9f43ae49e884a1b9be7dc5d6f9369ce>
+    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </DossierOwner>
+    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gd3cfa1af6a84b6687f5776992485533>
+    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF78F3BA-2CB7-4081-98E3-62DAC42A3FA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4724,4 +4688,38 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v0.56 Upgraded details inv val
</commit_message>
<xml_diff>
--- a/DEMO/DEMO_INT_EXT_25.xlsx
+++ b/DEMO/DEMO_INT_EXT_25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\I2E\DEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60C89A0-331F-4122-8E39-C8594E6A4773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C62E38A-A8B2-4843-B52B-F161851D868C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="497" xr2:uid="{0C90C80C-76BB-42B7-B048-59A6DFE1D745}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="99">
   <si>
     <t>Week starts on</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>Archie Bunker</t>
+  </si>
+  <si>
+    <t>PRO0023366</t>
   </si>
 </sst>
 </file>
@@ -855,8 +858,8 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,281 +1011,283 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
-        <v>45775</v>
+        <v>45663</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H4" s="11">
-        <v>100</v>
+        <v>750</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
-        <v>45782</v>
+        <v>45670</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H5" s="11">
-        <v>200</v>
+        <v>900</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
-        <v>45915</v>
+        <v>45677</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="9">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H6" s="11">
-        <v>300</v>
+        <v>1050</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
-        <v>45922</v>
+        <v>45684</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="9">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H7" s="11">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
-        <v>45985</v>
+        <v>45691</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="9">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H8" s="11">
-        <v>1300</v>
+        <v>4500</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
-        <v>45992</v>
+        <v>45712</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="9">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H9" s="11">
-        <v>1400</v>
+        <v>1440</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
-        <v>45845</v>
+        <v>45719</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F10" s="9">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="1">
-        <f>1300*1</f>
-        <v>1300</v>
+        <v>56</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1560</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>93</v>
@@ -1293,35 +1298,37 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
-        <v>45852</v>
+        <v>45726</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F11" s="9">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="1">
-        <f>1500*1</f>
-        <v>1500</v>
+        <v>57</v>
+      </c>
+      <c r="H11" s="11">
+        <v>50</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>93</v>
@@ -1331,44 +1338,44 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
-        <v>45592</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>37</v>
+      <c r="A12" s="29">
+        <v>45733</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="14">
-        <v>50</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="16">
-        <v>2000</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="9">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="11">
+        <v>100</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1379,7 +1386,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>26</v>
@@ -1388,19 +1395,19 @@
         <v>11</v>
       </c>
       <c r="F13" s="14">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="16">
-        <v>480</v>
+        <v>2000</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>88</v>
@@ -1420,7 +1427,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>26</v>
@@ -1429,16 +1436,16 @@
         <v>11</v>
       </c>
       <c r="F14" s="14">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="16">
-        <v>1500</v>
+        <v>480</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>28</v>
@@ -1461,7 +1468,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>26</v>
@@ -1470,19 +1477,19 @@
         <v>11</v>
       </c>
       <c r="F15" s="14">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H15" s="16">
-        <v>6200</v>
+        <v>1500</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>88</v>
@@ -1502,7 +1509,7 @@
         <v>37</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>26</v>
@@ -1511,19 +1518,19 @@
         <v>11</v>
       </c>
       <c r="F16" s="14">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="16">
-        <v>3040</v>
+        <v>6200</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>88</v>
@@ -1543,7 +1550,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>26</v>
@@ -1552,19 +1559,19 @@
         <v>11</v>
       </c>
       <c r="F17" s="14">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="16">
-        <v>3150</v>
+        <v>3040</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>88</v>
@@ -1584,7 +1591,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>26</v>
@@ -1593,19 +1600,19 @@
         <v>11</v>
       </c>
       <c r="F18" s="14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="16">
-        <v>3300</v>
+        <v>3150</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>88</v>
@@ -1618,161 +1625,161 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
-        <v>45663</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>38</v>
+      <c r="A19" s="30">
+        <v>45592</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="9">
-        <v>10</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="11">
-        <v>750</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="14">
+        <v>22</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="16">
+        <v>3300</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
-        <v>45670</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>44</v>
+        <v>45324</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F20" s="9">
+        <v>80</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2000</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="11">
-        <v>900</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="J20" s="12" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
-        <v>45677</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>44</v>
+        <v>45324</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F21" s="9">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H21" s="11">
-        <v>1050</v>
+        <v>5000</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
-        <v>45740</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>45</v>
+        <v>45334</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F22" s="9">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H22" s="11">
-        <v>450</v>
+        <v>2300</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>93</v>
@@ -1783,10 +1790,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
-        <v>45747</v>
+        <v>45775</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>33</v>
@@ -1798,22 +1805,22 @@
         <v>50</v>
       </c>
       <c r="F23" s="9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="11">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>93</v>
@@ -1824,37 +1831,37 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
-        <v>45887</v>
+        <v>45782</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" s="9">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="11">
-        <v>1875</v>
+        <v>200</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>93</v>
@@ -1865,34 +1872,34 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
-        <v>45894</v>
+        <v>45740</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="9">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H25" s="11">
-        <v>2175</v>
+        <v>450</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>87</v>
@@ -1906,34 +1913,34 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
-        <v>45957</v>
+        <v>45747</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F26" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H26" s="11">
-        <v>675</v>
+        <v>600</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>87</v>
@@ -1947,40 +1954,40 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>45964</v>
+        <v>45754</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F27" s="9">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H27" s="11">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M27" s="10" t="s">
         <v>96</v>
@@ -1988,115 +1995,119 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
-        <v>45817</v>
+        <v>45761</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="F28" s="9">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="1">
-        <f>525*1</f>
-        <v>525</v>
+        <v>55</v>
+      </c>
+      <c r="H28" s="11">
+        <v>7500</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
-        <v>45824</v>
+        <v>45768</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="F29" s="9">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="1">
-        <f>600*1</f>
-        <v>600</v>
+        <v>55</v>
+      </c>
+      <c r="H29" s="11">
+        <v>6750</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
-        <v>45324</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>27</v>
+        <v>45789</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F30" s="9">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="H30" s="11">
-        <v>2000</v>
+        <v>180</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>93</v>
@@ -2107,92 +2118,92 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
-        <v>45684</v>
+        <v>45796</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F31" s="9">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H31" s="11">
-        <v>4000</v>
+        <v>240</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
-        <v>45691</v>
+        <v>45803</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F32" s="9">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H32" s="11">
-        <v>4500</v>
+        <v>125</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
-        <v>45754</v>
+        <v>45810</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>33</v>
@@ -2204,25 +2215,25 @@
         <v>50</v>
       </c>
       <c r="F33" s="9">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H33" s="11">
-        <v>7000</v>
+        <v>150</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M33" s="10" t="s">
         <v>96</v>
@@ -2230,40 +2241,40 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
-        <v>45761</v>
+        <v>45915</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F34" s="9">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H34" s="11">
-        <v>7500</v>
+        <v>300</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>96</v>
@@ -2271,40 +2282,40 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="29">
-        <v>45768</v>
+        <v>45922</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F35" s="9">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H35" s="11">
-        <v>6750</v>
+        <v>400</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M35" s="10" t="s">
         <v>96</v>
@@ -2312,10 +2323,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
-        <v>45901</v>
+        <v>45887</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>35</v>
@@ -2327,25 +2338,25 @@
         <v>51</v>
       </c>
       <c r="F36" s="9">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H36" s="11">
-        <v>250</v>
+        <v>1875</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M36" s="10" t="s">
         <v>96</v>
@@ -2353,10 +2364,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
-        <v>45908</v>
+        <v>45894</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>35</v>
@@ -2368,25 +2379,25 @@
         <v>51</v>
       </c>
       <c r="F37" s="9">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H37" s="11">
-        <v>500</v>
+        <v>2175</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M37" s="10" t="s">
         <v>96</v>
@@ -2394,34 +2405,34 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
-        <v>45971</v>
+        <v>45901</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F38" s="9">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G38" s="10" t="s">
         <v>55</v>
       </c>
       <c r="H38" s="11">
-        <v>2750</v>
+        <v>250</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>85</v>
@@ -2435,34 +2446,34 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
-        <v>45978</v>
+        <v>45908</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39" s="9">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>55</v>
       </c>
       <c r="H39" s="11">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="K39" s="10" t="s">
         <v>85</v>
@@ -2476,114 +2487,119 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
-        <v>45831</v>
+        <v>45929</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="F40" s="9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H40" s="1">
-        <f>2250*1</f>
-        <v>2250</v>
+        <v>56</v>
+      </c>
+      <c r="H40" s="11">
+        <v>300</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
-        <v>45838</v>
+        <v>45936</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="F41" s="9">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H41" s="11">
-        <v>2750</v>
+        <v>360</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
-        <v>45324</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>27</v>
+        <v>45950</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F42" s="9">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H42" s="11">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>93</v>
@@ -2594,37 +2610,37 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
-        <v>45334</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>27</v>
+        <v>45943</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F43" s="9">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="H43" s="11">
-        <v>2300</v>
+        <v>175</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>93</v>
@@ -2635,119 +2651,119 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
-        <v>45712</v>
+        <v>45985</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F44" s="9">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H44" s="11">
-        <v>1440</v>
+        <v>1300</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
-        <v>45719</v>
+        <v>45992</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F45" s="9">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H45" s="11">
-        <v>1560</v>
+        <v>1400</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
-        <v>45789</v>
+        <v>45957</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F46" s="9">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H46" s="11">
-        <v>180</v>
+        <v>675</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>93</v>
@@ -2758,37 +2774,37 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
-        <v>45796</v>
+        <v>45964</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F47" s="9">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H47" s="11">
-        <v>240</v>
+        <v>750</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>93</v>
@@ -2799,40 +2815,40 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
-        <v>45929</v>
+        <v>45971</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F48" s="9">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="11">
-        <v>300</v>
+        <v>2750</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M48" s="10" t="s">
         <v>96</v>
@@ -2840,40 +2856,40 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
-        <v>45936</v>
+        <v>45978</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F49" s="9">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" s="11">
-        <v>360</v>
+        <v>3000</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M49" s="10" t="s">
         <v>96</v>
@@ -2963,113 +2979,115 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
-        <v>45859</v>
+        <v>46013</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F52" s="9">
         <v>17</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H52" s="11">
-        <v>1020</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H52" s="1"/>
       <c r="I52" s="12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J52" s="12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="29">
-        <v>45866</v>
+        <v>46020</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F53" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H53" s="11">
-        <v>1140</v>
-      </c>
-      <c r="I53" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J53" s="12" t="s">
-        <v>63</v>
+        <v>450</v>
+      </c>
+      <c r="I53" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>58</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
-        <v>45726</v>
+        <v>45845</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F54" s="9">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H54" s="11">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="H54" s="1">
+        <f>1300*1</f>
+        <v>1300</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J54" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>93</v>
@@ -3080,37 +3098,35 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="29">
-        <v>45733</v>
+        <v>45852</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F55" s="9">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H55" s="11">
-        <v>100</v>
+        <v>53</v>
+      </c>
+      <c r="H55" s="1">
+        <f>1500*1</f>
+        <v>1500</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>93</v>
@@ -3121,69 +3137,65 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
-        <v>45803</v>
+        <v>45817</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F56" s="9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H56" s="11">
-        <v>125</v>
+        <v>54</v>
+      </c>
+      <c r="H56" s="1">
+        <f>525*1</f>
+        <v>525</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="29">
-        <v>45810</v>
+        <v>45824</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F57" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H57" s="11">
-        <v>150</v>
+        <v>54</v>
+      </c>
+      <c r="H57" s="1">
+        <f>600*1</f>
+        <v>600</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>62</v>
@@ -3192,175 +3204,166 @@
         <v>62</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M57" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
-        <v>45950</v>
+        <v>45831</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F58" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H58" s="11">
-        <v>200</v>
+        <v>55</v>
+      </c>
+      <c r="H58" s="1">
+        <f>2250*1</f>
+        <v>2250</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L58" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M58" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="29">
-        <v>45943</v>
+        <v>45838</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F59" s="9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H59" s="11">
-        <v>175</v>
+        <v>2750</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L59" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M59" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
-        <v>46013</v>
+        <v>45859</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F60" s="9">
         <v>17</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H60" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="H60" s="11">
+        <v>1020</v>
+      </c>
       <c r="I60" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M60" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
-        <v>46020</v>
+        <v>45866</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F61" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H61" s="11">
-        <v>450</v>
-      </c>
-      <c r="I61" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="J61" s="31" t="s">
-        <v>58</v>
+        <v>1140</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>93</v>
       </c>
       <c r="M61" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3442,7 +3445,7 @@
   </sheetData>
   <autoFilter ref="A1:M63" xr:uid="{71860C13-2C7C-4F48-80B3-9582C9C756CA}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M63">
-      <sortCondition ref="B1:B63"/>
+      <sortCondition ref="D1:D63"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4274,6 +4277,99 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
+      <Description>RPRC6KRT5W67-1044406188-39062</Description>
+    </_dlc_DocIdUrl>
+    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g9f43ae49e884a1b9be7dc5d6f9369ce>
+    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </DossierOwner>
+    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </gd3cfa1af6a84b6687f5776992485533>
+    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FFB3B7DE9242943AFC83F55587E815F" ma:contentTypeVersion="332" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa82c5eea78b7e638bce7457d0c1ee6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f1f29378-94b6-4af4-bdac-5601381a5dad" xmlns:ns3="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="361f62c40be1fed3631387308499c1cb" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4577,100 +4673,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">RPRC6KRT5W67-1044406188-39062</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Url>https://allianzms.sharepoint.com/teams/BE0002-3408239-PMO-Benelux/_layouts/15/DocIdRedir.aspx?ID=RPRC6KRT5W67-1044406188-39062</Url>
-      <Description>RPRC6KRT5W67-1044406188-39062</Description>
-    </_dlc_DocIdUrl>
-    <MailPreviewData xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ContractExpirationDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <g9f43ae49e884a1b9be7dc5d6f9369ce xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g9f43ae49e884a1b9be7dc5d6f9369ce>
-    <DossierStatus xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <TaxCatchAllLabel xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <DossierOwner xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </DossierOwner>
-    <gd3cfa1af6a84b6687f5776992485533 xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </gd3cfa1af6a84b6687f5776992485533>
-    <_dlc_DocIdPersistId xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-    <ContractDate xmlns="7ec26cd4-2880-4894-b4b0-70aff63a2a6a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF78F3BA-2CB7-4081-98E3-62DAC42A3FA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4688,38 +4725,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F19100-E5F4-48BB-BC85-BF882D3E0D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B806233-07FC-4729-B591-BAF557312197}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDED237F-D2D1-467B-B55A-01FC7A4029C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ec26cd4-2880-4894-b4b0-70aff63a2a6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f1f29378-94b6-4af4-bdac-5601381a5dad"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>